<commit_message>
[aep.xlsx] excel data for aep demo
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/Aep/aep.xlsx
+++ b/src/test/resources/excelData/Aep/aep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\SeleniumFramework\src\test\resources\excelData\Honda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\SeleniumFramework\src\test\resources\excelData\Aep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42372568-887B-4654-A239-7E460EE7AED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313A1436-200E-48FB-A42A-FEF039CFE38F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -175,12 +175,6 @@
     <t>SystemOption</t>
   </si>
   <si>
-    <t>com.google.android.dialer</t>
-  </si>
-  <si>
-    <t>.extensions.GoogleDialtactsActivity</t>
-  </si>
-  <si>
     <t>android</t>
   </si>
   <si>
@@ -194,6 +188,15 @@
   </si>
   <si>
     <t>desktopIe</t>
+  </si>
+  <si>
+    <t>apeUser</t>
+  </si>
+  <si>
+    <t>aepUser</t>
+  </si>
+  <si>
+    <t>aepPassword</t>
   </si>
 </sst>
 </file>
@@ -784,18 +787,18 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -901,13 +904,13 @@
         <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>32</v>
@@ -936,13 +939,13 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>33</v>
@@ -971,7 +974,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1006,13 +1009,13 @@
         <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>35</v>
@@ -1044,7 +1047,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1068,7 +1071,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1097,7 +1100,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1108,19 +1111,21 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="N9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="S9" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
     </row>
@@ -1132,7 +1137,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1163,7 +1168,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>

</xml_diff>

<commit_message>
[aep.xlsx] update test data
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/Aep/aep.xlsx
+++ b/src/test/resources/excelData/Aep/aep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\SeleniumFramework\src\test\resources\excelData\Aep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313A1436-200E-48FB-A42A-FEF039CFE38F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62505F2B-372E-44CA-B8C0-99D09231884E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>desktopIe</t>
-  </si>
-  <si>
-    <t>apeUser</t>
   </si>
   <si>
     <t>aepUser</t>
@@ -775,7 +772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2D1F1-7BA5-4534-88B6-D969E332B0E1}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1115,10 +1114,10 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>

</xml_diff>